<commit_message>
Importing Excel Sheet Used Batch Insert
</commit_message>
<xml_diff>
--- a/backend/web/uploads/branches_file.xlsx
+++ b/backend/web/uploads/branches_file.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>branch_id</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>active</t>
-  </si>
-  <si>
-    <t>2017-03-24  12:03:49'</t>
   </si>
 </sst>
 </file>
@@ -403,7 +400,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,8 +446,8 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+      <c r="E2" s="1">
+        <v>42818.502650462964</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>

</xml_diff>